<commit_message>
feat: re-construct i18n dic
</commit_message>
<xml_diff>
--- a/src/data/i18n/i18n.xlsx
+++ b/src/data/i18n/i18n.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\WebApp\YgkTool\src\data\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA68D2C-43DD-47F6-B503-AABE8B3EBD1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80EFBB9-457F-4943-B545-4399D9371207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,6 +76,26 @@
   </si>
   <si>
     <t>图片视频</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>homePage.meta.title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Home</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>云极客工具，励志做最轻盈最好用的在线工具。以工匠精神打造功能丰富的在线工具，无需下载即可免费使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>homePage.meta.description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -423,7 +443,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -451,49 +471,59 @@
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
@@ -623,6 +653,9 @@
     <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E6">
+    <sortCondition ref="A1:A6"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>